<commit_message>
adding object oriented code for data observability
</commit_message>
<xml_diff>
--- a/Accelerator/Data Observability/Output/client_month_dim.xlsx
+++ b/Accelerator/Data Observability/Output/client_month_dim.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Numerical" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Categorical" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Drift" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Drift" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Numerical" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Categorical" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,10 +18,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -39,12 +46,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -57,14 +79,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -427,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,69 +462,19 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Datatype</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Zeros</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Negatives</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Missing Values</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>% Missing Values</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Unique Values</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Minimum</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Maximum</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Mean</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Median</t>
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>column</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>mean_drift</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>std_drift</t>
         </is>
       </c>
     </row>
@@ -508,45 +484,11 @@
           <t>client_id</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>float64</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Continuous</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>261576</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>5140</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>15158</v>
-      </c>
-      <c r="L2" t="n">
-        <v>4940.5</v>
-      </c>
-      <c r="M2" t="n">
-        <v>3880</v>
+      <c r="B2" t="n">
+        <v>1012.66491546839</v>
+      </c>
+      <c r="C2" t="n">
+        <v>658.5296660213448</v>
       </c>
     </row>
     <row r="3">
@@ -555,45 +497,11 @@
           <t>fsv_till_date</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>float64</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Continuous</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>261576</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2974</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>35841</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>2591575.18</v>
-      </c>
-      <c r="L3" t="n">
-        <v>24194.42</v>
-      </c>
-      <c r="M3" t="n">
-        <v>8440</v>
+      <c r="B3" t="n">
+        <v>3228.382646720402</v>
+      </c>
+      <c r="C3" t="n">
+        <v>12445.68268808133</v>
       </c>
     </row>
     <row r="4">
@@ -602,45 +510,11 @@
           <t>ir_till_date</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>float64</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Continuous</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>261576</v>
-      </c>
-      <c r="E4" t="n">
-        <v>16671</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>25266</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>978978.85</v>
-      </c>
-      <c r="L4" t="n">
-        <v>12650.19</v>
-      </c>
-      <c r="M4" t="n">
-        <v>4094.5</v>
+      <c r="B4" t="n">
+        <v>1596.4503655152</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5251.216566400715</v>
       </c>
     </row>
     <row r="5">
@@ -649,45 +523,11 @@
           <t>fsv</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>float64</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Continuous</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>261576</v>
-      </c>
-      <c r="E5" t="n">
-        <v>191959</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>10465</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1463608.75</v>
-      </c>
-      <c r="L5" t="n">
-        <v>728.85</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
+      <c r="B5" t="n">
+        <v>95.30517104602336</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1821.877509902018</v>
       </c>
     </row>
     <row r="6">
@@ -696,45 +536,11 @@
           <t>ir</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>float64</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Continuous</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>261576</v>
-      </c>
-      <c r="E6" t="n">
-        <v>217831</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>8916</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>151522</v>
-      </c>
-      <c r="L6" t="n">
-        <v>300.86</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
+      <c r="B6" t="n">
+        <v>51.14976339411101</v>
+      </c>
+      <c r="C6" t="n">
+        <v>40.50959388513411</v>
       </c>
     </row>
   </sheetData>
@@ -748,7 +554,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -757,77 +563,245 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Datatype</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Zeros</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Negatives</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Missing Values</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>% Missing Values</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Unique Values</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Mode</t>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Minimum</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>Maximum</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>Median</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>status_on_date</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
+          <t>client_id</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>265328</v>
       </c>
       <c r="C2" t="n">
-        <v>18043</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>243533</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>93.09999999999999</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Inactive</t>
-        </is>
+        <v>5304</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>15663</v>
+      </c>
+      <c r="J2" t="n">
+        <v>5083.19</v>
+      </c>
+      <c r="K2" t="n">
+        <v>4017</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>fsv_till_date</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>265328</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3166</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>36489</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2613077.74</v>
+      </c>
+      <c r="J3" t="n">
+        <v>24274.36</v>
+      </c>
+      <c r="K3" t="n">
+        <v>8432.68</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ir_till_date</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>265328</v>
+      </c>
+      <c r="C4" t="n">
+        <v>16900</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>25977</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>984026.05</v>
+      </c>
+      <c r="J4" t="n">
+        <v>12807.21</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4090.75</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>fsv</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>265328</v>
+      </c>
+      <c r="C5" t="n">
+        <v>194067</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>10681</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1463608.75</v>
+      </c>
+      <c r="J5" t="n">
+        <v>740.27</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ir</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>265328</v>
+      </c>
+      <c r="C6" t="n">
+        <v>220414</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>9223</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>153620</v>
+      </c>
+      <c r="J6" t="n">
+        <v>311</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -841,14 +815,79 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Zeros</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Missing Values</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>% Missing Values</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Unique Values</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Mode</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>status_on_date</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>18043</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>247285</v>
+      </c>
+      <c r="E2" t="n">
+        <v>93.2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>